<commit_message>
Fix Error: Remove Data Validation from Place of Supply Column
</commit_message>
<xml_diff>
--- a/E2TGST/Resources/PurchaseEntries.xlsx
+++ b/E2TGST/Resources/PurchaseEntries.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Dineshkumar\Projects\Excel-to-Tally-for-GST\E2TGST\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Excel-to-Tally-for-GST\E2TGST\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7B860959-8642-45B3-A339-EC02EC46D01E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Purchase Entries" sheetId="1" r:id="rId1"/>
@@ -90,7 +91,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -228,22 +229,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M1000" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:M1000"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:M1000" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A1:M1000" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="GSTN" dataDxfId="12"/>
-    <tableColumn id="2" name="Invoice No" dataDxfId="11"/>
-    <tableColumn id="3" name="Invoice Date" dataDxfId="10"/>
-    <tableColumn id="4" name="Invoice Value" dataDxfId="9"/>
-    <tableColumn id="5" name="GST Rate" dataDxfId="8"/>
-    <tableColumn id="6" name="Taxable Value" dataDxfId="7"/>
-    <tableColumn id="7" name="IGST" dataDxfId="6"/>
-    <tableColumn id="8" name="CGST" dataDxfId="5"/>
-    <tableColumn id="9" name="SGST" dataDxfId="4"/>
-    <tableColumn id="10" name="CESS" dataDxfId="3"/>
-    <tableColumn id="11" name="Ledger Name" dataDxfId="2"/>
-    <tableColumn id="12" name="Voucher Type" dataDxfId="1"/>
-    <tableColumn id="13" name="Place of Supply" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="GSTN" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Invoice No" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Invoice Date" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Invoice Value" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="GST Rate" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Taxable Value" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="IGST" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="CGST" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="SGST" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="CESS" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Ledger Name" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Voucher Type" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Place of Supply" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -511,12 +512,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="PurchaseEntries"/>
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3575,7 +3576,7 @@
       <c r="M1000" s="4"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="K2PsfzFVkmXXoY67eMHjHpnRgohaQ8XlZ2RmNTuwB142bqMZLG9jFAUM8amEk3iLpB0VxzuFhyznWWoAJ/G0VQ==" saltValue="PqOH78f29XIe1XO+tilzLA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0" insertRows="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="6zROMAbTTrWBB0qRd9yN252e4FQhD0rbxi7s1keNNR5Y9d1IF0STevxf36zoPu5s0tmLTVOk/KQJyqfk9i8Dcw==" saltValue="KnAEldUfaD4K4gTXK5hsAQ==" spinCount="100000" sheet="1" formatColumns="0" insertRows="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
@@ -3584,13 +3585,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Lists!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:M1000</xm:sqref>
+          <xm:sqref>L2:L1000</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$6</xm:f>
           </x14:formula1>
@@ -3603,7 +3604,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Lists"/>
   <dimension ref="A1:B6"/>
   <sheetViews>

</xml_diff>